<commit_message>
campo detalle importar -prueba
</commit_message>
<xml_diff>
--- a/public/formatos/formato_grupal.xlsx
+++ b/public/formatos/formato_grupal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/vaziko/public/formatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE3C274-D90D-E14D-AC08-AF9D7F7E1AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C738EFF0-9128-F245-994C-853E2F57A573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>01</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>NUMERO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>DESCRIPCION DOCUMENTO</t>
+  </si>
+  <si>
+    <t>Descripcion de prueba</t>
   </si>
 </sst>
 </file>
@@ -153,12 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0543E5F1-F206-3342-BD80-031D0C9A25F8}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -485,15 +492,16 @@
     <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
     <col min="6" max="7" width="23.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
-    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
-    <col min="12" max="14" width="10.83203125" style="1"/>
-    <col min="15" max="15" width="43.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="14.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="1" customWidth="1"/>
+    <col min="13" max="15" width="10.83203125" style="1"/>
+    <col min="16" max="16" width="43.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -515,30 +523,33 @@
       <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -560,86 +571,89 @@
       <c r="G2" s="1">
         <v>1204120120</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
         <v>72733</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I3" s="1" t="s">
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
+      <c r="L3" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
         <v>31171</v>
       </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I4" s="1" t="s">
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
         <v>5923</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I5" s="1" t="s">
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
+      <c r="L5" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
       <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
         <v>109827</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -658,182 +672,183 @@
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="5"/>
+      <c r="J6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>41224</v>
       </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I7" s="1" t="s">
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>42873</v>
       </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I8" s="1" t="s">
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>12991</v>
       </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I9" s="1" t="s">
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>15462</v>
       </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I10" s="1" t="s">
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>31678</v>
       </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I11" s="1" t="s">
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>40314</v>
       </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I12" s="1" t="s">
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>21123</v>
       </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I13" s="1" t="s">
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>34676</v>
       </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I14" s="1" t="s">
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
       <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
         <v>240341</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambios importar asientos -prueba
</commit_message>
<xml_diff>
--- a/public/formatos/formato_grupal.xlsx
+++ b/public/formatos/formato_grupal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/vaziko/public/formatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C738EFF0-9128-F245-994C-853E2F57A573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8048BC-610F-0F4C-AD55-2ACC1DADEAE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
   <si>
     <t>01</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Descripcion de prueba</t>
+  </si>
+  <si>
+    <t>ORDEN</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0543E5F1-F206-3342-BD80-031D0C9A25F8}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -496,12 +499,12 @@
     <col min="9" max="9" width="12.33203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="1"/>
     <col min="11" max="11" width="14.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" style="1" customWidth="1"/>
-    <col min="13" max="15" width="10.83203125" style="1"/>
-    <col min="16" max="16" width="43.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="43.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -534,22 +537,25 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -577,83 +583,83 @@
       <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
+      <c r="M2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
         <v>72733</v>
       </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
+      <c r="M3" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
         <v>31171</v>
       </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
+      <c r="M4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
         <v>5923</v>
       </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
+      <c r="M5" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
         <v>109827</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -676,179 +682,179 @@
       <c r="J6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>41224</v>
       </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>42873</v>
       </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>12991</v>
       </c>
-      <c r="O8" s="1">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>15462</v>
       </c>
-      <c r="O9" s="1">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>31678</v>
       </c>
-      <c r="O10" s="1">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>40314</v>
       </c>
-      <c r="O11" s="1">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>21123</v>
       </c>
-      <c r="O12" s="1">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>34676</v>
       </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
       <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
         <v>240341</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambios formato grupal -prueba
</commit_message>
<xml_diff>
--- a/public/formatos/formato_grupal.xlsx
+++ b/public/formatos/formato_grupal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/vaziko/public/formatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8048BC-610F-0F4C-AD55-2ACC1DADEAE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7BF837-F4E9-D341-94E8-AC63AD08FD28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>01</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>ORDEN</t>
+  </si>
+  <si>
+    <t>OP-00</t>
+  </si>
+  <si>
+    <t>999-99</t>
+  </si>
+  <si>
+    <t>FC-00</t>
   </si>
 </sst>
 </file>
@@ -486,7 +495,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,6 +592,12 @@
       <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="M2" s="1" t="s">
         <v>21</v>
       </c>
@@ -622,6 +637,12 @@
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>21</v>

</xml_diff>